<commit_message>
implement running without user interface
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Models\AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B64BAED-FBAA-4325-A735-FA2D6E133BF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="5484" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="5484" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>parameter</t>
   </si>
@@ -180,12 +181,24 @@
   </si>
   <si>
     <t>program_perc_culture_coverage</t>
+  </si>
+  <si>
+    <t>riskgroup_perc_hiv</t>
+  </si>
+  <si>
+    <t>riskgroup_perc_urbanpoor</t>
+  </si>
+  <si>
+    <t>riskgroup_perc_ruralpoor</t>
+  </si>
+  <si>
+    <t>riskgroup_perc_prison</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -1206,669 +1219,669 @@
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma" xfId="663" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="614"/>
-    <cellStyle name="Comma 2 2" xfId="626"/>
-    <cellStyle name="Input 2" xfId="378"/>
+    <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma 2 2" xfId="626" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Input 2" xfId="378" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="545"/>
-    <cellStyle name="Normal 2" xfId="449"/>
-    <cellStyle name="Normal 2 2" xfId="439"/>
-    <cellStyle name="Normal 3" xfId="448"/>
-    <cellStyle name="Normal 3 2" xfId="500"/>
-    <cellStyle name="Normal 4" xfId="451"/>
-    <cellStyle name="Normal 4 2" xfId="81"/>
-    <cellStyle name="Normal 5" xfId="450"/>
-    <cellStyle name="Normal 5 2" xfId="242"/>
-    <cellStyle name="Normal 6" xfId="453"/>
-    <cellStyle name="Normal 6 10" xfId="41"/>
-    <cellStyle name="Normal 6 10 2" xfId="121"/>
-    <cellStyle name="Normal 6 10 2 2" xfId="168"/>
-    <cellStyle name="Normal 6 10 2 3" xfId="167"/>
-    <cellStyle name="Normal 6 10 3" xfId="118"/>
-    <cellStyle name="Normal 6 10 4" xfId="117"/>
-    <cellStyle name="Normal 6 11" xfId="40"/>
-    <cellStyle name="Normal 6 11 2" xfId="251"/>
-    <cellStyle name="Normal 6 11 2 2" xfId="421"/>
-    <cellStyle name="Normal 6 11 2 3" xfId="422"/>
-    <cellStyle name="Normal 6 11 3" xfId="252"/>
-    <cellStyle name="Normal 6 11 4" xfId="250"/>
-    <cellStyle name="Normal 6 12" xfId="43"/>
-    <cellStyle name="Normal 6 12 2" xfId="227"/>
-    <cellStyle name="Normal 6 12 2 2" xfId="181"/>
-    <cellStyle name="Normal 6 12 2 3" xfId="180"/>
-    <cellStyle name="Normal 6 12 3" xfId="226"/>
-    <cellStyle name="Normal 6 12 4" xfId="225"/>
-    <cellStyle name="Normal 6 13" xfId="42"/>
-    <cellStyle name="Normal 6 13 2" xfId="16"/>
-    <cellStyle name="Normal 6 13 2 2" xfId="503"/>
-    <cellStyle name="Normal 6 13 2 3" xfId="504"/>
-    <cellStyle name="Normal 6 13 3" xfId="17"/>
-    <cellStyle name="Normal 6 13 4" xfId="11"/>
-    <cellStyle name="Normal 6 14" xfId="45"/>
-    <cellStyle name="Normal 6 14 2" xfId="337"/>
-    <cellStyle name="Normal 6 14 2 2" xfId="76"/>
-    <cellStyle name="Normal 6 14 2 3" xfId="75"/>
-    <cellStyle name="Normal 6 14 3" xfId="336"/>
-    <cellStyle name="Normal 6 14 4" xfId="338"/>
-    <cellStyle name="Normal 6 15" xfId="44"/>
-    <cellStyle name="Normal 6 15 2" xfId="130"/>
-    <cellStyle name="Normal 6 15 3" xfId="131"/>
-    <cellStyle name="Normal 6 16" xfId="47"/>
-    <cellStyle name="Normal 6 17" xfId="46"/>
-    <cellStyle name="Normal 6 2" xfId="315"/>
-    <cellStyle name="Normal 6 2 10" xfId="233"/>
-    <cellStyle name="Normal 6 2 11" xfId="232"/>
-    <cellStyle name="Normal 6 2 2" xfId="578"/>
-    <cellStyle name="Normal 6 2 2 10" xfId="528"/>
-    <cellStyle name="Normal 6 2 2 2" xfId="465"/>
-    <cellStyle name="Normal 6 2 2 2 2" xfId="485"/>
-    <cellStyle name="Normal 6 2 2 2 2 2" xfId="512"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2" xfId="7"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2 2" xfId="329"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2 3" xfId="328"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 3" xfId="6"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 4" xfId="8"/>
-    <cellStyle name="Normal 6 2 2 2 2 3" xfId="511"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2" xfId="218"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2 2" xfId="67"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2 3" xfId="68"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 3" xfId="219"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 4" xfId="220"/>
-    <cellStyle name="Normal 6 2 2 2 2 4" xfId="309"/>
-    <cellStyle name="Normal 6 2 2 2 2 4 2" xfId="437"/>
-    <cellStyle name="Normal 6 2 2 2 2 4 3" xfId="436"/>
-    <cellStyle name="Normal 6 2 2 2 2 5" xfId="260"/>
-    <cellStyle name="Normal 6 2 2 2 2 6" xfId="508"/>
-    <cellStyle name="Normal 6 2 2 2 3" xfId="191"/>
-    <cellStyle name="Normal 6 2 2 2 3 2" xfId="56"/>
-    <cellStyle name="Normal 6 2 2 2 3 2 2" xfId="496"/>
-    <cellStyle name="Normal 6 2 2 2 3 2 3" xfId="497"/>
-    <cellStyle name="Normal 6 2 2 2 3 3" xfId="57"/>
-    <cellStyle name="Normal 6 2 2 2 3 4" xfId="54"/>
-    <cellStyle name="Normal 6 2 2 2 4" xfId="178"/>
-    <cellStyle name="Normal 6 2 2 2 4 2" xfId="385"/>
-    <cellStyle name="Normal 6 2 2 2 4 2 2" xfId="73"/>
-    <cellStyle name="Normal 6 2 2 2 4 2 3" xfId="71"/>
-    <cellStyle name="Normal 6 2 2 2 4 3" xfId="384"/>
-    <cellStyle name="Normal 6 2 2 2 4 4" xfId="389"/>
-    <cellStyle name="Normal 6 2 2 2 5" xfId="177"/>
-    <cellStyle name="Normal 6 2 2 2 5 2" xfId="592"/>
-    <cellStyle name="Normal 6 2 2 2 5 3" xfId="593"/>
-    <cellStyle name="Normal 6 2 2 2 6" xfId="483"/>
-    <cellStyle name="Normal 6 2 2 2 7" xfId="482"/>
-    <cellStyle name="Normal 6 2 2 3" xfId="464"/>
-    <cellStyle name="Normal 6 2 2 3 2" xfId="24"/>
-    <cellStyle name="Normal 6 2 2 3 2 2" xfId="230"/>
-    <cellStyle name="Normal 6 2 2 3 2 2 2" xfId="560"/>
-    <cellStyle name="Normal 6 2 2 3 2 2 3" xfId="561"/>
-    <cellStyle name="Normal 6 2 2 3 2 3" xfId="231"/>
-    <cellStyle name="Normal 6 2 2 3 2 4" xfId="228"/>
-    <cellStyle name="Normal 6 2 2 3 3" xfId="25"/>
-    <cellStyle name="Normal 6 2 2 3 3 2" xfId="31"/>
-    <cellStyle name="Normal 6 2 2 3 3 2 2" xfId="133"/>
-    <cellStyle name="Normal 6 2 2 3 3 2 3" xfId="132"/>
-    <cellStyle name="Normal 6 2 2 3 3 3" xfId="30"/>
-    <cellStyle name="Normal 6 2 2 3 3 4" xfId="27"/>
-    <cellStyle name="Normal 6 2 2 3 4" xfId="20"/>
-    <cellStyle name="Normal 6 2 2 3 4 2" xfId="193"/>
-    <cellStyle name="Normal 6 2 2 3 4 3" xfId="194"/>
-    <cellStyle name="Normal 6 2 2 3 5" xfId="21"/>
-    <cellStyle name="Normal 6 2 2 3 6" xfId="22"/>
-    <cellStyle name="Normal 6 2 2 4" xfId="467"/>
-    <cellStyle name="Normal 6 2 2 4 2" xfId="206"/>
-    <cellStyle name="Normal 6 2 2 4 2 2" xfId="143"/>
-    <cellStyle name="Normal 6 2 2 4 2 3" xfId="544"/>
-    <cellStyle name="Normal 6 2 2 4 3" xfId="205"/>
-    <cellStyle name="Normal 6 2 2 4 4" xfId="533"/>
-    <cellStyle name="Normal 6 2 2 5" xfId="466"/>
-    <cellStyle name="Normal 6 2 2 5 2" xfId="405"/>
-    <cellStyle name="Normal 6 2 2 5 2 2" xfId="248"/>
-    <cellStyle name="Normal 6 2 2 5 2 3" xfId="249"/>
-    <cellStyle name="Normal 6 2 2 5 3" xfId="406"/>
-    <cellStyle name="Normal 6 2 2 5 4" xfId="408"/>
-    <cellStyle name="Normal 6 2 2 6" xfId="469"/>
-    <cellStyle name="Normal 6 2 2 6 2" xfId="602"/>
-    <cellStyle name="Normal 6 2 2 6 2 2" xfId="590"/>
-    <cellStyle name="Normal 6 2 2 6 2 3" xfId="589"/>
-    <cellStyle name="Normal 6 2 2 6 3" xfId="601"/>
-    <cellStyle name="Normal 6 2 2 6 4" xfId="603"/>
-    <cellStyle name="Normal 6 2 2 7" xfId="468"/>
-    <cellStyle name="Normal 6 2 2 7 2" xfId="156"/>
-    <cellStyle name="Normal 6 2 2 7 2 2" xfId="262"/>
-    <cellStyle name="Normal 6 2 2 7 2 3" xfId="263"/>
-    <cellStyle name="Normal 6 2 2 7 3" xfId="157"/>
-    <cellStyle name="Normal 6 2 2 7 4" xfId="158"/>
-    <cellStyle name="Normal 6 2 2 8" xfId="101"/>
-    <cellStyle name="Normal 6 2 2 8 2" xfId="349"/>
-    <cellStyle name="Normal 6 2 2 8 3" xfId="348"/>
-    <cellStyle name="Normal 6 2 2 9" xfId="99"/>
-    <cellStyle name="Normal 6 2 3" xfId="577"/>
-    <cellStyle name="Normal 6 2 3 2" xfId="12"/>
-    <cellStyle name="Normal 6 2 3 2 2" xfId="294"/>
-    <cellStyle name="Normal 6 2 3 2 2 2" xfId="360"/>
-    <cellStyle name="Normal 6 2 3 2 2 2 2" xfId="526"/>
-    <cellStyle name="Normal 6 2 3 2 2 2 3" xfId="527"/>
-    <cellStyle name="Normal 6 2 3 2 2 3" xfId="361"/>
-    <cellStyle name="Normal 6 2 3 2 2 4" xfId="355"/>
-    <cellStyle name="Normal 6 2 3 2 3" xfId="295"/>
-    <cellStyle name="Normal 6 2 3 2 3 2" xfId="173"/>
-    <cellStyle name="Normal 6 2 3 2 3 2 2" xfId="443"/>
-    <cellStyle name="Normal 6 2 3 2 3 2 3" xfId="442"/>
-    <cellStyle name="Normal 6 2 3 2 3 3" xfId="172"/>
-    <cellStyle name="Normal 6 2 3 2 3 4" xfId="169"/>
-    <cellStyle name="Normal 6 2 3 2 4" xfId="289"/>
-    <cellStyle name="Normal 6 2 3 2 4 2" xfId="213"/>
-    <cellStyle name="Normal 6 2 3 2 4 3" xfId="214"/>
-    <cellStyle name="Normal 6 2 3 2 5" xfId="290"/>
-    <cellStyle name="Normal 6 2 3 2 6" xfId="291"/>
-    <cellStyle name="Normal 6 2 3 3" xfId="13"/>
-    <cellStyle name="Normal 6 2 3 3 2" xfId="84"/>
-    <cellStyle name="Normal 6 2 3 3 2 2" xfId="543"/>
-    <cellStyle name="Normal 6 2 3 3 2 3" xfId="542"/>
-    <cellStyle name="Normal 6 2 3 3 3" xfId="83"/>
-    <cellStyle name="Normal 6 2 3 3 4" xfId="82"/>
-    <cellStyle name="Normal 6 2 3 4" xfId="14"/>
-    <cellStyle name="Normal 6 2 3 4 2" xfId="216"/>
-    <cellStyle name="Normal 6 2 3 4 2 2" xfId="660"/>
-    <cellStyle name="Normal 6 2 3 4 2 3" xfId="661"/>
-    <cellStyle name="Normal 6 2 3 4 3" xfId="55"/>
-    <cellStyle name="Normal 6 2 3 4 4" xfId="223"/>
-    <cellStyle name="Normal 6 2 3 5" xfId="15"/>
-    <cellStyle name="Normal 6 2 3 5 2" xfId="506"/>
-    <cellStyle name="Normal 6 2 3 5 3" xfId="505"/>
-    <cellStyle name="Normal 6 2 3 6" xfId="69"/>
-    <cellStyle name="Normal 6 2 3 7" xfId="72"/>
-    <cellStyle name="Normal 6 2 4" xfId="331"/>
-    <cellStyle name="Normal 6 2 4 2" xfId="400"/>
-    <cellStyle name="Normal 6 2 4 2 2" xfId="256"/>
-    <cellStyle name="Normal 6 2 4 2 2 2" xfId="274"/>
-    <cellStyle name="Normal 6 2 4 2 2 3" xfId="270"/>
-    <cellStyle name="Normal 6 2 4 2 3" xfId="255"/>
-    <cellStyle name="Normal 6 2 4 2 4" xfId="257"/>
-    <cellStyle name="Normal 6 2 4 3" xfId="399"/>
-    <cellStyle name="Normal 6 2 4 3 2" xfId="458"/>
-    <cellStyle name="Normal 6 2 4 3 2 2" xfId="150"/>
-    <cellStyle name="Normal 6 2 4 3 2 3" xfId="151"/>
-    <cellStyle name="Normal 6 2 4 3 3" xfId="459"/>
-    <cellStyle name="Normal 6 2 4 3 4" xfId="463"/>
-    <cellStyle name="Normal 6 2 4 4" xfId="398"/>
-    <cellStyle name="Normal 6 2 4 4 2" xfId="522"/>
-    <cellStyle name="Normal 6 2 4 4 3" xfId="521"/>
-    <cellStyle name="Normal 6 2 4 5" xfId="397"/>
-    <cellStyle name="Normal 6 2 4 6" xfId="396"/>
-    <cellStyle name="Normal 6 2 5" xfId="330"/>
-    <cellStyle name="Normal 6 2 5 2" xfId="569"/>
-    <cellStyle name="Normal 6 2 5 2 2" xfId="376"/>
-    <cellStyle name="Normal 6 2 5 2 3" xfId="377"/>
-    <cellStyle name="Normal 6 2 5 3" xfId="570"/>
-    <cellStyle name="Normal 6 2 5 4" xfId="568"/>
-    <cellStyle name="Normal 6 2 6" xfId="333"/>
-    <cellStyle name="Normal 6 2 6 2" xfId="632"/>
-    <cellStyle name="Normal 6 2 6 2 2" xfId="175"/>
-    <cellStyle name="Normal 6 2 6 2 3" xfId="174"/>
-    <cellStyle name="Normal 6 2 6 3" xfId="631"/>
-    <cellStyle name="Normal 6 2 6 4" xfId="630"/>
-    <cellStyle name="Normal 6 2 7" xfId="332"/>
-    <cellStyle name="Normal 6 2 7 2" xfId="195"/>
-    <cellStyle name="Normal 6 2 7 2 2" xfId="635"/>
-    <cellStyle name="Normal 6 2 7 2 3" xfId="636"/>
-    <cellStyle name="Normal 6 2 7 3" xfId="196"/>
-    <cellStyle name="Normal 6 2 7 4" xfId="427"/>
-    <cellStyle name="Normal 6 2 8" xfId="335"/>
-    <cellStyle name="Normal 6 2 8 2" xfId="474"/>
-    <cellStyle name="Normal 6 2 8 2 2" xfId="524"/>
-    <cellStyle name="Normal 6 2 8 2 3" xfId="523"/>
-    <cellStyle name="Normal 6 2 8 3" xfId="473"/>
-    <cellStyle name="Normal 6 2 8 4" xfId="479"/>
-    <cellStyle name="Normal 6 2 9" xfId="334"/>
-    <cellStyle name="Normal 6 2 9 2" xfId="26"/>
-    <cellStyle name="Normal 6 2 9 3" xfId="98"/>
-    <cellStyle name="Normal 6 3" xfId="314"/>
-    <cellStyle name="Normal 6 3 10" xfId="183"/>
-    <cellStyle name="Normal 6 3 2" xfId="548"/>
-    <cellStyle name="Normal 6 3 2 2" xfId="207"/>
-    <cellStyle name="Normal 6 3 2 2 2" xfId="237"/>
-    <cellStyle name="Normal 6 3 2 2 2 2" xfId="50"/>
-    <cellStyle name="Normal 6 3 2 2 2 2 2" xfId="89"/>
-    <cellStyle name="Normal 6 3 2 2 2 2 3" xfId="90"/>
-    <cellStyle name="Normal 6 3 2 2 2 3" xfId="51"/>
-    <cellStyle name="Normal 6 3 2 2 2 4" xfId="48"/>
-    <cellStyle name="Normal 6 3 2 2 3" xfId="238"/>
-    <cellStyle name="Normal 6 3 2 2 3 2" xfId="499"/>
-    <cellStyle name="Normal 6 3 2 2 3 2 2" xfId="288"/>
-    <cellStyle name="Normal 6 3 2 2 3 2 3" xfId="287"/>
-    <cellStyle name="Normal 6 3 2 2 3 3" xfId="498"/>
-    <cellStyle name="Normal 6 3 2 2 3 4" xfId="495"/>
-    <cellStyle name="Normal 6 3 2 2 4" xfId="234"/>
-    <cellStyle name="Normal 6 3 2 2 4 2" xfId="612"/>
-    <cellStyle name="Normal 6 3 2 2 4 3" xfId="613"/>
-    <cellStyle name="Normal 6 3 2 2 5" xfId="235"/>
-    <cellStyle name="Normal 6 3 2 2 6" xfId="236"/>
-    <cellStyle name="Normal 6 3 2 3" xfId="208"/>
-    <cellStyle name="Normal 6 3 2 3 2" xfId="37"/>
-    <cellStyle name="Normal 6 3 2 3 2 2" xfId="394"/>
-    <cellStyle name="Normal 6 3 2 3 2 3" xfId="393"/>
-    <cellStyle name="Normal 6 3 2 3 3" xfId="36"/>
-    <cellStyle name="Normal 6 3 2 3 4" xfId="35"/>
-    <cellStyle name="Normal 6 3 2 4" xfId="209"/>
-    <cellStyle name="Normal 6 3 2 4 2" xfId="627"/>
-    <cellStyle name="Normal 6 3 2 4 2 2" xfId="486"/>
-    <cellStyle name="Normal 6 3 2 4 2 3" xfId="487"/>
-    <cellStyle name="Normal 6 3 2 4 3" xfId="628"/>
-    <cellStyle name="Normal 6 3 2 4 4" xfId="629"/>
-    <cellStyle name="Normal 6 3 2 5" xfId="210"/>
-    <cellStyle name="Normal 6 3 2 5 2" xfId="431"/>
-    <cellStyle name="Normal 6 3 2 5 3" xfId="430"/>
-    <cellStyle name="Normal 6 3 2 6" xfId="211"/>
-    <cellStyle name="Normal 6 3 2 7" xfId="212"/>
-    <cellStyle name="Normal 6 3 3" xfId="549"/>
-    <cellStyle name="Normal 6 3 3 2" xfId="645"/>
-    <cellStyle name="Normal 6 3 3 2 2" xfId="558"/>
-    <cellStyle name="Normal 6 3 3 2 2 2" xfId="190"/>
-    <cellStyle name="Normal 6 3 3 2 2 3" xfId="189"/>
-    <cellStyle name="Normal 6 3 3 2 3" xfId="557"/>
-    <cellStyle name="Normal 6 3 3 2 4" xfId="556"/>
-    <cellStyle name="Normal 6 3 3 3" xfId="644"/>
-    <cellStyle name="Normal 6 3 3 3 2" xfId="114"/>
-    <cellStyle name="Normal 6 3 3 3 2 2" xfId="653"/>
-    <cellStyle name="Normal 6 3 3 3 2 3" xfId="654"/>
-    <cellStyle name="Normal 6 3 3 3 3" xfId="115"/>
-    <cellStyle name="Normal 6 3 3 3 4" xfId="112"/>
-    <cellStyle name="Normal 6 3 3 4" xfId="647"/>
-    <cellStyle name="Normal 6 3 3 4 2" xfId="317"/>
-    <cellStyle name="Normal 6 3 3 4 3" xfId="316"/>
-    <cellStyle name="Normal 6 3 3 5" xfId="646"/>
-    <cellStyle name="Normal 6 3 3 6" xfId="648"/>
-    <cellStyle name="Normal 6 3 4" xfId="550"/>
-    <cellStyle name="Normal 6 3 4 2" xfId="160"/>
-    <cellStyle name="Normal 6 3 4 2 2" xfId="470"/>
-    <cellStyle name="Normal 6 3 4 2 3" xfId="471"/>
-    <cellStyle name="Normal 6 3 4 3" xfId="164"/>
-    <cellStyle name="Normal 6 3 4 4" xfId="155"/>
-    <cellStyle name="Normal 6 3 5" xfId="551"/>
-    <cellStyle name="Normal 6 3 5 2" xfId="493"/>
-    <cellStyle name="Normal 6 3 5 2 2" xfId="53"/>
-    <cellStyle name="Normal 6 3 5 2 3" xfId="52"/>
-    <cellStyle name="Normal 6 3 5 3" xfId="492"/>
-    <cellStyle name="Normal 6 3 5 4" xfId="491"/>
-    <cellStyle name="Normal 6 3 6" xfId="552"/>
-    <cellStyle name="Normal 6 3 6 2" xfId="323"/>
-    <cellStyle name="Normal 6 3 6 2 2" xfId="153"/>
-    <cellStyle name="Normal 6 3 6 2 3" xfId="154"/>
-    <cellStyle name="Normal 6 3 6 3" xfId="324"/>
-    <cellStyle name="Normal 6 3 6 4" xfId="322"/>
-    <cellStyle name="Normal 6 3 7" xfId="553"/>
-    <cellStyle name="Normal 6 3 7 2" xfId="111"/>
-    <cellStyle name="Normal 6 3 7 2 2" xfId="347"/>
-    <cellStyle name="Normal 6 3 7 2 3" xfId="346"/>
-    <cellStyle name="Normal 6 3 7 3" xfId="110"/>
-    <cellStyle name="Normal 6 3 7 4" xfId="109"/>
-    <cellStyle name="Normal 6 3 8" xfId="501"/>
-    <cellStyle name="Normal 6 3 8 2" xfId="305"/>
-    <cellStyle name="Normal 6 3 8 3" xfId="306"/>
-    <cellStyle name="Normal 6 3 9" xfId="502"/>
-    <cellStyle name="Normal 6 4" xfId="311"/>
-    <cellStyle name="Normal 6 4 10" xfId="100"/>
-    <cellStyle name="Normal 6 4 2" xfId="92"/>
-    <cellStyle name="Normal 6 4 2 2" xfId="140"/>
-    <cellStyle name="Normal 6 4 2 2 2" xfId="375"/>
-    <cellStyle name="Normal 6 4 2 2 2 2" xfId="267"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="382"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 3" xfId="381"/>
-    <cellStyle name="Normal 6 4 2 2 2 3" xfId="266"/>
-    <cellStyle name="Normal 6 4 2 2 2 4" xfId="268"/>
-    <cellStyle name="Normal 6 4 2 2 3" xfId="395"/>
-    <cellStyle name="Normal 6 4 2 2 3 2" xfId="480"/>
-    <cellStyle name="Normal 6 4 2 2 3 2 2" xfId="187"/>
-    <cellStyle name="Normal 6 4 2 2 3 2 3" xfId="188"/>
-    <cellStyle name="Normal 6 4 2 2 3 3" xfId="481"/>
-    <cellStyle name="Normal 6 4 2 2 3 4" xfId="484"/>
-    <cellStyle name="Normal 6 4 2 2 4" xfId="402"/>
-    <cellStyle name="Normal 6 4 2 2 4 2" xfId="429"/>
-    <cellStyle name="Normal 6 4 2 2 4 3" xfId="428"/>
-    <cellStyle name="Normal 6 4 2 2 5" xfId="401"/>
-    <cellStyle name="Normal 6 4 2 2 6" xfId="379"/>
-    <cellStyle name="Normal 6 4 2 3" xfId="139"/>
-    <cellStyle name="Normal 6 4 2 3 2" xfId="587"/>
-    <cellStyle name="Normal 6 4 2 3 2 2" xfId="655"/>
-    <cellStyle name="Normal 6 4 2 3 2 3" xfId="656"/>
-    <cellStyle name="Normal 6 4 2 3 3" xfId="588"/>
-    <cellStyle name="Normal 6 4 2 3 4" xfId="591"/>
-    <cellStyle name="Normal 6 4 2 4" xfId="138"/>
-    <cellStyle name="Normal 6 4 2 4 2" xfId="623"/>
-    <cellStyle name="Normal 6 4 2 4 2 2" xfId="605"/>
-    <cellStyle name="Normal 6 4 2 4 2 3" xfId="604"/>
-    <cellStyle name="Normal 6 4 2 4 3" xfId="622"/>
-    <cellStyle name="Normal 6 4 2 4 4" xfId="621"/>
-    <cellStyle name="Normal 6 4 2 5" xfId="137"/>
-    <cellStyle name="Normal 6 4 2 5 2" xfId="184"/>
-    <cellStyle name="Normal 6 4 2 5 3" xfId="185"/>
-    <cellStyle name="Normal 6 4 2 6" xfId="136"/>
-    <cellStyle name="Normal 6 4 2 7" xfId="135"/>
-    <cellStyle name="Normal 6 4 3" xfId="91"/>
-    <cellStyle name="Normal 6 4 3 2" xfId="342"/>
-    <cellStyle name="Normal 6 4 3 2 2" xfId="200"/>
-    <cellStyle name="Normal 6 4 3 2 2 2" xfId="127"/>
-    <cellStyle name="Normal 6 4 3 2 2 3" xfId="128"/>
-    <cellStyle name="Normal 6 4 3 2 3" xfId="201"/>
-    <cellStyle name="Normal 6 4 3 2 4" xfId="204"/>
-    <cellStyle name="Normal 6 4 3 3" xfId="343"/>
-    <cellStyle name="Normal 6 4 3 3 2" xfId="643"/>
-    <cellStyle name="Normal 6 4 3 3 2 2" xfId="298"/>
-    <cellStyle name="Normal 6 4 3 3 2 3" xfId="297"/>
-    <cellStyle name="Normal 6 4 3 3 3" xfId="642"/>
-    <cellStyle name="Normal 6 4 3 3 4" xfId="583"/>
-    <cellStyle name="Normal 6 4 3 4" xfId="340"/>
-    <cellStyle name="Normal 6 4 3 4 2" xfId="444"/>
-    <cellStyle name="Normal 6 4 3 4 3" xfId="445"/>
-    <cellStyle name="Normal 6 4 3 5" xfId="341"/>
-    <cellStyle name="Normal 6 4 3 6" xfId="339"/>
-    <cellStyle name="Normal 6 4 4" xfId="441"/>
-    <cellStyle name="Normal 6 4 4 2" xfId="292"/>
-    <cellStyle name="Normal 6 4 4 2 2" xfId="247"/>
-    <cellStyle name="Normal 6 4 4 2 3" xfId="246"/>
-    <cellStyle name="Normal 6 4 4 3" xfId="412"/>
-    <cellStyle name="Normal 6 4 4 4" xfId="293"/>
-    <cellStyle name="Normal 6 4 5" xfId="440"/>
-    <cellStyle name="Normal 6 4 5 2" xfId="460"/>
-    <cellStyle name="Normal 6 4 5 2 2" xfId="517"/>
-    <cellStyle name="Normal 6 4 5 2 3" xfId="520"/>
-    <cellStyle name="Normal 6 4 5 3" xfId="461"/>
-    <cellStyle name="Normal 6 4 5 4" xfId="462"/>
-    <cellStyle name="Normal 6 4 6" xfId="88"/>
-    <cellStyle name="Normal 6 4 6 2" xfId="5"/>
-    <cellStyle name="Normal 6 4 6 2 2" xfId="595"/>
-    <cellStyle name="Normal 6 4 6 2 3" xfId="594"/>
-    <cellStyle name="Normal 6 4 6 3" xfId="4"/>
-    <cellStyle name="Normal 6 4 6 4" xfId="10"/>
-    <cellStyle name="Normal 6 4 7" xfId="87"/>
-    <cellStyle name="Normal 6 4 7 2" xfId="221"/>
-    <cellStyle name="Normal 6 4 7 2 2" xfId="403"/>
-    <cellStyle name="Normal 6 4 7 2 3" xfId="404"/>
-    <cellStyle name="Normal 6 4 7 3" xfId="222"/>
-    <cellStyle name="Normal 6 4 7 4" xfId="224"/>
-    <cellStyle name="Normal 6 4 8" xfId="97"/>
-    <cellStyle name="Normal 6 4 8 2" xfId="95"/>
-    <cellStyle name="Normal 6 4 8 3" xfId="380"/>
-    <cellStyle name="Normal 6 4 9" xfId="96"/>
-    <cellStyle name="Normal 6 5" xfId="310"/>
-    <cellStyle name="Normal 6 5 2" xfId="285"/>
-    <cellStyle name="Normal 6 5 2 2" xfId="534"/>
-    <cellStyle name="Normal 6 5 2 2 2" xfId="182"/>
-    <cellStyle name="Normal 6 5 2 2 2 2" xfId="258"/>
-    <cellStyle name="Normal 6 5 2 2 2 2 2" xfId="546"/>
-    <cellStyle name="Normal 6 5 2 2 2 2 3" xfId="547"/>
-    <cellStyle name="Normal 6 5 2 2 2 3" xfId="259"/>
-    <cellStyle name="Normal 6 5 2 2 2 4" xfId="261"/>
-    <cellStyle name="Normal 6 5 2 2 3" xfId="417"/>
-    <cellStyle name="Normal 6 5 2 2 3 2" xfId="302"/>
-    <cellStyle name="Normal 6 5 2 2 3 2 2" xfId="107"/>
-    <cellStyle name="Normal 6 5 2 2 3 2 3" xfId="106"/>
-    <cellStyle name="Normal 6 5 2 2 3 3" xfId="301"/>
-    <cellStyle name="Normal 6 5 2 2 3 4" xfId="79"/>
-    <cellStyle name="Normal 6 5 2 2 4" xfId="253"/>
-    <cellStyle name="Normal 6 5 2 2 4 2" xfId="419"/>
-    <cellStyle name="Normal 6 5 2 2 4 3" xfId="420"/>
-    <cellStyle name="Normal 6 5 2 2 5" xfId="254"/>
-    <cellStyle name="Normal 6 5 2 2 6" xfId="192"/>
-    <cellStyle name="Normal 6 5 2 3" xfId="535"/>
-    <cellStyle name="Normal 6 5 2 3 2" xfId="649"/>
-    <cellStyle name="Normal 6 5 2 3 2 2" xfId="370"/>
-    <cellStyle name="Normal 6 5 2 3 2 3" xfId="369"/>
-    <cellStyle name="Normal 6 5 2 3 3" xfId="70"/>
-    <cellStyle name="Normal 6 5 2 3 4" xfId="276"/>
-    <cellStyle name="Normal 6 5 2 4" xfId="532"/>
-    <cellStyle name="Normal 6 5 2 4 2" xfId="518"/>
-    <cellStyle name="Normal 6 5 2 4 2 2" xfId="633"/>
-    <cellStyle name="Normal 6 5 2 4 2 3" xfId="634"/>
-    <cellStyle name="Normal 6 5 2 4 3" xfId="519"/>
-    <cellStyle name="Normal 6 5 2 4 4" xfId="514"/>
-    <cellStyle name="Normal 6 5 2 5" xfId="447"/>
-    <cellStyle name="Normal 6 5 2 5 2" xfId="304"/>
-    <cellStyle name="Normal 6 5 2 5 3" xfId="303"/>
-    <cellStyle name="Normal 6 5 2 6" xfId="530"/>
-    <cellStyle name="Normal 6 5 2 7" xfId="531"/>
-    <cellStyle name="Normal 6 5 3" xfId="286"/>
-    <cellStyle name="Normal 6 5 3 2" xfId="321"/>
-    <cellStyle name="Normal 6 5 3 2 2" xfId="134"/>
-    <cellStyle name="Normal 6 5 3 2 2 2" xfId="600"/>
-    <cellStyle name="Normal 6 5 3 2 2 3" xfId="599"/>
-    <cellStyle name="Normal 6 5 3 2 3" xfId="229"/>
-    <cellStyle name="Normal 6 5 3 2 4" xfId="472"/>
-    <cellStyle name="Normal 6 5 3 3" xfId="320"/>
-    <cellStyle name="Normal 6 5 3 3 2" xfId="32"/>
-    <cellStyle name="Normal 6 5 3 3 2 2" xfId="423"/>
-    <cellStyle name="Normal 6 5 3 3 2 3" xfId="424"/>
-    <cellStyle name="Normal 6 5 3 3 3" xfId="34"/>
-    <cellStyle name="Normal 6 5 3 3 4" xfId="9"/>
-    <cellStyle name="Normal 6 5 3 4" xfId="319"/>
-    <cellStyle name="Normal 6 5 3 4 2" xfId="94"/>
-    <cellStyle name="Normal 6 5 3 4 3" xfId="93"/>
-    <cellStyle name="Normal 6 5 3 5" xfId="318"/>
-    <cellStyle name="Normal 6 5 3 6" xfId="525"/>
-    <cellStyle name="Normal 6 5 4" xfId="283"/>
-    <cellStyle name="Normal 6 5 4 2" xfId="582"/>
-    <cellStyle name="Normal 6 5 4 2 2" xfId="478"/>
-    <cellStyle name="Normal 6 5 4 2 3" xfId="639"/>
-    <cellStyle name="Normal 6 5 4 3" xfId="197"/>
-    <cellStyle name="Normal 6 5 4 4" xfId="584"/>
-    <cellStyle name="Normal 6 5 5" xfId="284"/>
-    <cellStyle name="Normal 6 5 5 2" xfId="387"/>
-    <cellStyle name="Normal 6 5 5 2 2" xfId="119"/>
-    <cellStyle name="Normal 6 5 5 2 3" xfId="33"/>
-    <cellStyle name="Normal 6 5 5 3" xfId="386"/>
-    <cellStyle name="Normal 6 5 5 4" xfId="388"/>
-    <cellStyle name="Normal 6 5 6" xfId="281"/>
-    <cellStyle name="Normal 6 5 6 2" xfId="74"/>
-    <cellStyle name="Normal 6 5 6 3" xfId="356"/>
-    <cellStyle name="Normal 6 5 7" xfId="282"/>
-    <cellStyle name="Normal 6 5 8" xfId="280"/>
-    <cellStyle name="Normal 6 6" xfId="313"/>
-    <cellStyle name="Normal 6 6 2" xfId="326"/>
-    <cellStyle name="Normal 6 6 2 2" xfId="245"/>
-    <cellStyle name="Normal 6 6 2 2 2" xfId="64"/>
-    <cellStyle name="Normal 6 6 2 2 2 2" xfId="618"/>
-    <cellStyle name="Normal 6 6 2 2 2 2 2" xfId="39"/>
-    <cellStyle name="Normal 6 6 2 2 2 2 3" xfId="515"/>
-    <cellStyle name="Normal 6 6 2 2 2 3" xfId="617"/>
-    <cellStyle name="Normal 6 6 2 2 2 4" xfId="619"/>
-    <cellStyle name="Normal 6 6 2 2 3" xfId="113"/>
-    <cellStyle name="Normal 6 6 2 2 3 2" xfId="116"/>
-    <cellStyle name="Normal 6 6 2 2 3 2 2" xfId="456"/>
-    <cellStyle name="Normal 6 6 2 2 3 2 3" xfId="457"/>
-    <cellStyle name="Normal 6 6 2 2 3 3" xfId="296"/>
-    <cellStyle name="Normal 6 6 2 2 3 4" xfId="176"/>
-    <cellStyle name="Normal 6 6 2 2 4" xfId="80"/>
-    <cellStyle name="Normal 6 6 2 2 4 2" xfId="199"/>
-    <cellStyle name="Normal 6 6 2 2 4 3" xfId="198"/>
-    <cellStyle name="Normal 6 6 2 2 5" xfId="77"/>
-    <cellStyle name="Normal 6 6 2 2 6" xfId="129"/>
-    <cellStyle name="Normal 6 6 2 3" xfId="163"/>
-    <cellStyle name="Normal 6 6 2 3 2" xfId="662"/>
-    <cellStyle name="Normal 6 6 2 3 2 2" xfId="278"/>
-    <cellStyle name="Normal 6 6 2 3 2 3" xfId="279"/>
-    <cellStyle name="Normal 6 6 2 3 3" xfId="1"/>
-    <cellStyle name="Normal 6 6 2 3 4" xfId="2"/>
-    <cellStyle name="Normal 6 6 2 4" xfId="586"/>
-    <cellStyle name="Normal 6 6 2 4 2" xfId="581"/>
-    <cellStyle name="Normal 6 6 2 4 2 2" xfId="383"/>
-    <cellStyle name="Normal 6 6 2 4 2 3" xfId="516"/>
-    <cellStyle name="Normal 6 6 2 4 3" xfId="580"/>
-    <cellStyle name="Normal 6 6 2 4 4" xfId="579"/>
-    <cellStyle name="Normal 6 6 2 5" xfId="159"/>
-    <cellStyle name="Normal 6 6 2 5 2" xfId="141"/>
-    <cellStyle name="Normal 6 6 2 5 3" xfId="142"/>
-    <cellStyle name="Normal 6 6 2 6" xfId="162"/>
-    <cellStyle name="Normal 6 6 2 7" xfId="161"/>
-    <cellStyle name="Normal 6 6 3" xfId="325"/>
-    <cellStyle name="Normal 6 6 3 2" xfId="374"/>
-    <cellStyle name="Normal 6 6 3 2 2" xfId="275"/>
-    <cellStyle name="Normal 6 6 3 2 2 2" xfId="410"/>
-    <cellStyle name="Normal 6 6 3 2 2 3" xfId="411"/>
-    <cellStyle name="Normal 6 6 3 2 3" xfId="362"/>
-    <cellStyle name="Normal 6 6 3 2 4" xfId="277"/>
-    <cellStyle name="Normal 6 6 3 3" xfId="186"/>
-    <cellStyle name="Normal 6 6 3 3 2" xfId="105"/>
-    <cellStyle name="Normal 6 6 3 3 2 2" xfId="300"/>
-    <cellStyle name="Normal 6 6 3 3 2 3" xfId="299"/>
-    <cellStyle name="Normal 6 6 3 3 3" xfId="104"/>
-    <cellStyle name="Normal 6 6 3 3 4" xfId="574"/>
-    <cellStyle name="Normal 6 6 3 4" xfId="371"/>
-    <cellStyle name="Normal 6 6 3 4 2" xfId="391"/>
-    <cellStyle name="Normal 6 6 3 4 3" xfId="392"/>
-    <cellStyle name="Normal 6 6 3 5" xfId="372"/>
-    <cellStyle name="Normal 6 6 3 6" xfId="373"/>
-    <cellStyle name="Normal 6 6 4" xfId="108"/>
-    <cellStyle name="Normal 6 6 4 2" xfId="435"/>
-    <cellStyle name="Normal 6 6 4 2 2" xfId="433"/>
-    <cellStyle name="Normal 6 6 4 2 3" xfId="432"/>
-    <cellStyle name="Normal 6 6 4 3" xfId="434"/>
-    <cellStyle name="Normal 6 6 4 4" xfId="438"/>
-    <cellStyle name="Normal 6 6 5" xfId="585"/>
-    <cellStyle name="Normal 6 6 5 2" xfId="596"/>
-    <cellStyle name="Normal 6 6 5 2 2" xfId="554"/>
-    <cellStyle name="Normal 6 6 5 2 3" xfId="555"/>
-    <cellStyle name="Normal 6 6 5 3" xfId="597"/>
-    <cellStyle name="Normal 6 6 5 4" xfId="598"/>
-    <cellStyle name="Normal 6 6 6" xfId="616"/>
-    <cellStyle name="Normal 6 6 6 2" xfId="29"/>
-    <cellStyle name="Normal 6 6 6 3" xfId="28"/>
-    <cellStyle name="Normal 6 6 7" xfId="507"/>
-    <cellStyle name="Normal 6 6 8" xfId="513"/>
-    <cellStyle name="Normal 6 7" xfId="312"/>
-    <cellStyle name="Normal 6 7 2" xfId="65"/>
-    <cellStyle name="Normal 6 7 2 2" xfId="610"/>
-    <cellStyle name="Normal 6 7 2 2 2" xfId="122"/>
-    <cellStyle name="Normal 6 7 2 2 2 2" xfId="615"/>
-    <cellStyle name="Normal 6 7 2 2 2 2 2" xfId="243"/>
-    <cellStyle name="Normal 6 7 2 2 2 2 3" xfId="244"/>
-    <cellStyle name="Normal 6 7 2 2 2 3" xfId="120"/>
-    <cellStyle name="Normal 6 7 2 2 2 4" xfId="562"/>
-    <cellStyle name="Normal 6 7 2 2 3" xfId="123"/>
-    <cellStyle name="Normal 6 7 2 2 3 2" xfId="358"/>
-    <cellStyle name="Normal 6 7 2 2 3 2 2" xfId="390"/>
-    <cellStyle name="Normal 6 7 2 2 3 2 3" xfId="144"/>
-    <cellStyle name="Normal 6 7 2 2 3 3" xfId="357"/>
-    <cellStyle name="Normal 6 7 2 2 3 4" xfId="359"/>
-    <cellStyle name="Normal 6 7 2 2 4" xfId="124"/>
-    <cellStyle name="Normal 6 7 2 2 4 2" xfId="170"/>
-    <cellStyle name="Normal 6 7 2 2 4 3" xfId="171"/>
-    <cellStyle name="Normal 6 7 2 2 5" xfId="125"/>
-    <cellStyle name="Normal 6 7 2 2 6" xfId="126"/>
-    <cellStyle name="Normal 6 7 2 3" xfId="611"/>
-    <cellStyle name="Normal 6 7 2 3 2" xfId="572"/>
-    <cellStyle name="Normal 6 7 2 3 2 2" xfId="49"/>
-    <cellStyle name="Normal 6 7 2 3 2 3" xfId="327"/>
-    <cellStyle name="Normal 6 7 2 3 3" xfId="571"/>
-    <cellStyle name="Normal 6 7 2 3 4" xfId="573"/>
-    <cellStyle name="Normal 6 7 2 4" xfId="606"/>
-    <cellStyle name="Normal 6 7 2 4 2" xfId="272"/>
-    <cellStyle name="Normal 6 7 2 4 2 2" xfId="179"/>
-    <cellStyle name="Normal 6 7 2 4 2 3" xfId="536"/>
-    <cellStyle name="Normal 6 7 2 4 3" xfId="273"/>
-    <cellStyle name="Normal 6 7 2 4 4" xfId="271"/>
-    <cellStyle name="Normal 6 7 2 5" xfId="607"/>
-    <cellStyle name="Normal 6 7 2 5 2" xfId="86"/>
-    <cellStyle name="Normal 6 7 2 5 3" xfId="85"/>
-    <cellStyle name="Normal 6 7 2 6" xfId="608"/>
-    <cellStyle name="Normal 6 7 2 7" xfId="609"/>
-    <cellStyle name="Normal 6 7 3" xfId="66"/>
-    <cellStyle name="Normal 6 7 3 2" xfId="409"/>
-    <cellStyle name="Normal 6 7 3 2 2" xfId="476"/>
-    <cellStyle name="Normal 6 7 3 2 2 2" xfId="353"/>
-    <cellStyle name="Normal 6 7 3 2 2 3" xfId="352"/>
-    <cellStyle name="Normal 6 7 3 2 3" xfId="475"/>
-    <cellStyle name="Normal 6 7 3 2 4" xfId="477"/>
-    <cellStyle name="Normal 6 7 3 3" xfId="418"/>
-    <cellStyle name="Normal 6 7 3 3 2" xfId="650"/>
-    <cellStyle name="Normal 6 7 3 3 2 2" xfId="19"/>
-    <cellStyle name="Normal 6 7 3 3 2 3" xfId="23"/>
-    <cellStyle name="Normal 6 7 3 3 3" xfId="651"/>
-    <cellStyle name="Normal 6 7 3 3 4" xfId="652"/>
-    <cellStyle name="Normal 6 7 3 4" xfId="414"/>
-    <cellStyle name="Normal 6 7 3 4 2" xfId="563"/>
-    <cellStyle name="Normal 6 7 3 4 3" xfId="620"/>
-    <cellStyle name="Normal 6 7 3 5" xfId="413"/>
-    <cellStyle name="Normal 6 7 3 6" xfId="407"/>
-    <cellStyle name="Normal 6 7 4" xfId="60"/>
-    <cellStyle name="Normal 6 7 4 2" xfId="166"/>
-    <cellStyle name="Normal 6 7 4 2 2" xfId="509"/>
-    <cellStyle name="Normal 6 7 4 2 3" xfId="510"/>
-    <cellStyle name="Normal 6 7 4 3" xfId="490"/>
-    <cellStyle name="Normal 6 7 4 4" xfId="494"/>
-    <cellStyle name="Normal 6 7 5" xfId="61"/>
-    <cellStyle name="Normal 6 7 5 2" xfId="638"/>
-    <cellStyle name="Normal 6 7 5 2 2" xfId="152"/>
-    <cellStyle name="Normal 6 7 5 2 3" xfId="38"/>
-    <cellStyle name="Normal 6 7 5 3" xfId="637"/>
-    <cellStyle name="Normal 6 7 5 4" xfId="641"/>
-    <cellStyle name="Normal 6 7 6" xfId="62"/>
-    <cellStyle name="Normal 6 7 6 2" xfId="415"/>
-    <cellStyle name="Normal 6 7 6 3" xfId="416"/>
-    <cellStyle name="Normal 6 7 7" xfId="63"/>
-    <cellStyle name="Normal 6 7 8" xfId="59"/>
-    <cellStyle name="Normal 6 8" xfId="308"/>
-    <cellStyle name="Normal 6 8 2" xfId="364"/>
-    <cellStyle name="Normal 6 8 2 2" xfId="146"/>
-    <cellStyle name="Normal 6 8 2 2 2" xfId="3"/>
-    <cellStyle name="Normal 6 8 2 2 2 2" xfId="345"/>
-    <cellStyle name="Normal 6 8 2 2 2 3" xfId="344"/>
-    <cellStyle name="Normal 6 8 2 2 3" xfId="18"/>
-    <cellStyle name="Normal 6 8 2 2 4" xfId="575"/>
-    <cellStyle name="Normal 6 8 2 3" xfId="145"/>
-    <cellStyle name="Normal 6 8 2 3 2" xfId="240"/>
-    <cellStyle name="Normal 6 8 2 3 2 2" xfId="202"/>
-    <cellStyle name="Normal 6 8 2 3 2 3" xfId="203"/>
-    <cellStyle name="Normal 6 8 2 3 3" xfId="241"/>
-    <cellStyle name="Normal 6 8 2 3 4" xfId="239"/>
-    <cellStyle name="Normal 6 8 2 4" xfId="149"/>
-    <cellStyle name="Normal 6 8 2 4 2" xfId="625"/>
-    <cellStyle name="Normal 6 8 2 4 3" xfId="624"/>
-    <cellStyle name="Normal 6 8 2 5" xfId="148"/>
-    <cellStyle name="Normal 6 8 2 6" xfId="147"/>
-    <cellStyle name="Normal 6 8 3" xfId="363"/>
-    <cellStyle name="Normal 6 8 3 2" xfId="350"/>
-    <cellStyle name="Normal 6 8 3 2 2" xfId="488"/>
-    <cellStyle name="Normal 6 8 3 2 3" xfId="489"/>
-    <cellStyle name="Normal 6 8 3 3" xfId="351"/>
-    <cellStyle name="Normal 6 8 3 4" xfId="354"/>
-    <cellStyle name="Normal 6 8 4" xfId="368"/>
-    <cellStyle name="Normal 6 8 4 2" xfId="565"/>
-    <cellStyle name="Normal 6 8 4 2 2" xfId="165"/>
-    <cellStyle name="Normal 6 8 4 2 3" xfId="446"/>
-    <cellStyle name="Normal 6 8 4 3" xfId="564"/>
-    <cellStyle name="Normal 6 8 4 4" xfId="559"/>
-    <cellStyle name="Normal 6 8 5" xfId="367"/>
-    <cellStyle name="Normal 6 8 5 2" xfId="102"/>
-    <cellStyle name="Normal 6 8 5 3" xfId="103"/>
-    <cellStyle name="Normal 6 8 6" xfId="366"/>
-    <cellStyle name="Normal 6 8 7" xfId="365"/>
-    <cellStyle name="Normal 6 9" xfId="307"/>
-    <cellStyle name="Normal 6 9 2" xfId="537"/>
-    <cellStyle name="Normal 6 9 2 2" xfId="215"/>
-    <cellStyle name="Normal 6 9 2 2 2" xfId="264"/>
-    <cellStyle name="Normal 6 9 2 2 3" xfId="265"/>
-    <cellStyle name="Normal 6 9 2 3" xfId="566"/>
-    <cellStyle name="Normal 6 9 2 4" xfId="217"/>
-    <cellStyle name="Normal 6 9 3" xfId="538"/>
-    <cellStyle name="Normal 6 9 3 2" xfId="658"/>
-    <cellStyle name="Normal 6 9 3 2 2" xfId="426"/>
-    <cellStyle name="Normal 6 9 3 2 3" xfId="425"/>
-    <cellStyle name="Normal 6 9 3 3" xfId="657"/>
-    <cellStyle name="Normal 6 9 3 4" xfId="659"/>
-    <cellStyle name="Normal 6 9 4" xfId="540"/>
-    <cellStyle name="Normal 6 9 4 2" xfId="640"/>
-    <cellStyle name="Normal 6 9 4 3" xfId="567"/>
-    <cellStyle name="Normal 6 9 5" xfId="541"/>
-    <cellStyle name="Normal 6 9 6" xfId="539"/>
-    <cellStyle name="Normal 7" xfId="452"/>
-    <cellStyle name="Normal 7 2" xfId="529"/>
-    <cellStyle name="Normal 8" xfId="455"/>
-    <cellStyle name="Normal 8 2" xfId="576"/>
-    <cellStyle name="Normal 9" xfId="454"/>
-    <cellStyle name="Normal 9 2" xfId="58"/>
-    <cellStyle name="Percent 2" xfId="269"/>
-    <cellStyle name="Percent 2 2" xfId="78"/>
+    <cellStyle name="Normal 10" xfId="545" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2" xfId="449" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2 2" xfId="439" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 3" xfId="448" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 3 2" xfId="500" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 4" xfId="451" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 4 2" xfId="81" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 5" xfId="450" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 5 2" xfId="242" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 6" xfId="453" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 6 10" xfId="41" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 6 10 2" xfId="121" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 6 10 2 2" xfId="168" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 6 10 2 3" xfId="167" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 6 10 3" xfId="118" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 6 10 4" xfId="117" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 6 11" xfId="40" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 6 11 2" xfId="251" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 6 11 2 2" xfId="421" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Normal 6 11 2 3" xfId="422" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Normal 6 11 3" xfId="252" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 6 11 4" xfId="250" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Normal 6 12" xfId="43" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 6 12 2" xfId="227" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal 6 12 2 2" xfId="181" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Normal 6 12 2 3" xfId="180" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 6 12 3" xfId="226" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Normal 6 12 4" xfId="225" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 6 13" xfId="42" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normal 6 13 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Normal 6 13 2 2" xfId="503" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Normal 6 13 2 3" xfId="504" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normal 6 13 3" xfId="17" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 6 13 4" xfId="11" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 6 14" xfId="45" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 6 14 2" xfId="337" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 6 14 2 2" xfId="76" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 6 14 2 3" xfId="75" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 6 14 3" xfId="336" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 6 14 4" xfId="338" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Normal 6 15" xfId="44" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Normal 6 15 2" xfId="130" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Normal 6 15 3" xfId="131" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 6 16" xfId="47" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Normal 6 17" xfId="46" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 6 2" xfId="315" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Normal 6 2 10" xfId="233" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Normal 6 2 11" xfId="232" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Normal 6 2 2" xfId="578" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Normal 6 2 2 10" xfId="528" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Normal 6 2 2 2" xfId="465" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2" xfId="485" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2" xfId="512" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2 2" xfId="329" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2 3" xfId="328" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 3" xfId="6" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 4" xfId="8" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3" xfId="511" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2" xfId="218" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2 3" xfId="68" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 3" xfId="219" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 4" xfId="220" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 4" xfId="309" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 4 2" xfId="437" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 4 3" xfId="436" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 5" xfId="260" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 6" xfId="508" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3" xfId="191" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 2" xfId="56" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 2 2" xfId="496" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 2 3" xfId="497" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 3" xfId="57" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 4" xfId="54" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4" xfId="178" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 2" xfId="385" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 2 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 2 3" xfId="71" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 3" xfId="384" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 4" xfId="389" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 6 2 2 2 5" xfId="177" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 6 2 2 2 5 2" xfId="592" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 6 2 2 2 5 3" xfId="593" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 6 2 2 2 6" xfId="483" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 6 2 2 2 7" xfId="482" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 6 2 2 3" xfId="464" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2" xfId="24" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 2" xfId="230" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 2 2" xfId="560" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 2 3" xfId="561" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 3" xfId="231" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 4" xfId="228" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3" xfId="25" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 2 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 2 3" xfId="132" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 3" xfId="30" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 4" xfId="27" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Normal 6 2 2 3 4" xfId="20" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Normal 6 2 2 3 4 2" xfId="193" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Normal 6 2 2 3 4 3" xfId="194" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Normal 6 2 2 3 5" xfId="21" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Normal 6 2 2 3 6" xfId="22" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Normal 6 2 2 4" xfId="467" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Normal 6 2 2 4 2" xfId="206" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Normal 6 2 2 4 2 2" xfId="143" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Normal 6 2 2 4 2 3" xfId="544" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Normal 6 2 2 4 3" xfId="205" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Normal 6 2 2 4 4" xfId="533" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Normal 6 2 2 5" xfId="466" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Normal 6 2 2 5 2" xfId="405" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Normal 6 2 2 5 2 2" xfId="248" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Normal 6 2 2 5 2 3" xfId="249" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Normal 6 2 2 5 3" xfId="406" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Normal 6 2 2 5 4" xfId="408" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Normal 6 2 2 6" xfId="469" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Normal 6 2 2 6 2" xfId="602" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Normal 6 2 2 6 2 2" xfId="590" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Normal 6 2 2 6 2 3" xfId="589" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Normal 6 2 2 6 3" xfId="601" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Normal 6 2 2 6 4" xfId="603" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Normal 6 2 2 7" xfId="468" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Normal 6 2 2 7 2" xfId="156" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Normal 6 2 2 7 2 2" xfId="262" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Normal 6 2 2 7 2 3" xfId="263" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Normal 6 2 2 7 3" xfId="157" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Normal 6 2 2 7 4" xfId="158" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Normal 6 2 2 8" xfId="101" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Normal 6 2 2 8 2" xfId="349" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Normal 6 2 2 8 3" xfId="348" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Normal 6 2 2 9" xfId="99" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Normal 6 2 3" xfId="577" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Normal 6 2 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2" xfId="294" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 2" xfId="360" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 2 2" xfId="526" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 2 3" xfId="527" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 3" xfId="361" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 4" xfId="355" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3" xfId="295" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 2" xfId="173" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 2 2" xfId="443" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 2 3" xfId="442" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 3" xfId="172" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 4" xfId="169" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Normal 6 2 3 2 4" xfId="289" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Normal 6 2 3 2 4 2" xfId="213" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Normal 6 2 3 2 4 3" xfId="214" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Normal 6 2 3 2 5" xfId="290" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Normal 6 2 3 2 6" xfId="291" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="Normal 6 2 3 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Normal 6 2 3 3 2" xfId="84" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="Normal 6 2 3 3 2 2" xfId="543" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Normal 6 2 3 3 2 3" xfId="542" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="Normal 6 2 3 3 3" xfId="83" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="Normal 6 2 3 3 4" xfId="82" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="Normal 6 2 3 4" xfId="14" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="Normal 6 2 3 4 2" xfId="216" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="Normal 6 2 3 4 2 2" xfId="660" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="Normal 6 2 3 4 2 3" xfId="661" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Normal 6 2 3 4 3" xfId="55" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Normal 6 2 3 4 4" xfId="223" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
+    <cellStyle name="Normal 6 2 3 5" xfId="15" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="Normal 6 2 3 5 2" xfId="506" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="Normal 6 2 3 5 3" xfId="505" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="Normal 6 2 3 6" xfId="69" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="Normal 6 2 3 7" xfId="72" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
+    <cellStyle name="Normal 6 2 4" xfId="331" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
+    <cellStyle name="Normal 6 2 4 2" xfId="400" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="Normal 6 2 4 2 2" xfId="256" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="Normal 6 2 4 2 2 2" xfId="274" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="Normal 6 2 4 2 2 3" xfId="270" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="Normal 6 2 4 2 3" xfId="255" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
+    <cellStyle name="Normal 6 2 4 2 4" xfId="257" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
+    <cellStyle name="Normal 6 2 4 3" xfId="399" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="Normal 6 2 4 3 2" xfId="458" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
+    <cellStyle name="Normal 6 2 4 3 2 2" xfId="150" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
+    <cellStyle name="Normal 6 2 4 3 2 3" xfId="151" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
+    <cellStyle name="Normal 6 2 4 3 3" xfId="459" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
+    <cellStyle name="Normal 6 2 4 3 4" xfId="463" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
+    <cellStyle name="Normal 6 2 4 4" xfId="398" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
+    <cellStyle name="Normal 6 2 4 4 2" xfId="522" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
+    <cellStyle name="Normal 6 2 4 4 3" xfId="521" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
+    <cellStyle name="Normal 6 2 4 5" xfId="397" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
+    <cellStyle name="Normal 6 2 4 6" xfId="396" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
+    <cellStyle name="Normal 6 2 5" xfId="330" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
+    <cellStyle name="Normal 6 2 5 2" xfId="569" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
+    <cellStyle name="Normal 6 2 5 2 2" xfId="376" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
+    <cellStyle name="Normal 6 2 5 2 3" xfId="377" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
+    <cellStyle name="Normal 6 2 5 3" xfId="570" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="Normal 6 2 5 4" xfId="568" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
+    <cellStyle name="Normal 6 2 6" xfId="333" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
+    <cellStyle name="Normal 6 2 6 2" xfId="632" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="Normal 6 2 6 2 2" xfId="175" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
+    <cellStyle name="Normal 6 2 6 2 3" xfId="174" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="Normal 6 2 6 3" xfId="631" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
+    <cellStyle name="Normal 6 2 6 4" xfId="630" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
+    <cellStyle name="Normal 6 2 7" xfId="332" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
+    <cellStyle name="Normal 6 2 7 2" xfId="195" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="Normal 6 2 7 2 2" xfId="635" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
+    <cellStyle name="Normal 6 2 7 2 3" xfId="636" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="Normal 6 2 7 3" xfId="196" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
+    <cellStyle name="Normal 6 2 7 4" xfId="427" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
+    <cellStyle name="Normal 6 2 8" xfId="335" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
+    <cellStyle name="Normal 6 2 8 2" xfId="474" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
+    <cellStyle name="Normal 6 2 8 2 2" xfId="524" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="Normal 6 2 8 2 3" xfId="523" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
+    <cellStyle name="Normal 6 2 8 3" xfId="473" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
+    <cellStyle name="Normal 6 2 8 4" xfId="479" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
+    <cellStyle name="Normal 6 2 9" xfId="334" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
+    <cellStyle name="Normal 6 2 9 2" xfId="26" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
+    <cellStyle name="Normal 6 2 9 3" xfId="98" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
+    <cellStyle name="Normal 6 3" xfId="314" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
+    <cellStyle name="Normal 6 3 10" xfId="183" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
+    <cellStyle name="Normal 6 3 2" xfId="548" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
+    <cellStyle name="Normal 6 3 2 2" xfId="207" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2" xfId="237" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 2 2" xfId="89" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 2 3" xfId="90" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 3" xfId="51" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 4" xfId="48" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3" xfId="238" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 2" xfId="499" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 2 2" xfId="288" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 2 3" xfId="287" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 3" xfId="498" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 4" xfId="495" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="Normal 6 3 2 2 4" xfId="234" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="Normal 6 3 2 2 4 2" xfId="612" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
+    <cellStyle name="Normal 6 3 2 2 4 3" xfId="613" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
+    <cellStyle name="Normal 6 3 2 2 5" xfId="235" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
+    <cellStyle name="Normal 6 3 2 2 6" xfId="236" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
+    <cellStyle name="Normal 6 3 2 3" xfId="208" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
+    <cellStyle name="Normal 6 3 2 3 2" xfId="37" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
+    <cellStyle name="Normal 6 3 2 3 2 2" xfId="394" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
+    <cellStyle name="Normal 6 3 2 3 2 3" xfId="393" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
+    <cellStyle name="Normal 6 3 2 3 3" xfId="36" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
+    <cellStyle name="Normal 6 3 2 3 4" xfId="35" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
+    <cellStyle name="Normal 6 3 2 4" xfId="209" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
+    <cellStyle name="Normal 6 3 2 4 2" xfId="627" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
+    <cellStyle name="Normal 6 3 2 4 2 2" xfId="486" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
+    <cellStyle name="Normal 6 3 2 4 2 3" xfId="487" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
+    <cellStyle name="Normal 6 3 2 4 3" xfId="628" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
+    <cellStyle name="Normal 6 3 2 4 4" xfId="629" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
+    <cellStyle name="Normal 6 3 2 5" xfId="210" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
+    <cellStyle name="Normal 6 3 2 5 2" xfId="431" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
+    <cellStyle name="Normal 6 3 2 5 3" xfId="430" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
+    <cellStyle name="Normal 6 3 2 6" xfId="211" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
+    <cellStyle name="Normal 6 3 2 7" xfId="212" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
+    <cellStyle name="Normal 6 3 3" xfId="549" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
+    <cellStyle name="Normal 6 3 3 2" xfId="645" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
+    <cellStyle name="Normal 6 3 3 2 2" xfId="558" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
+    <cellStyle name="Normal 6 3 3 2 2 2" xfId="190" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
+    <cellStyle name="Normal 6 3 3 2 2 3" xfId="189" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
+    <cellStyle name="Normal 6 3 3 2 3" xfId="557" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
+    <cellStyle name="Normal 6 3 3 2 4" xfId="556" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
+    <cellStyle name="Normal 6 3 3 3" xfId="644" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
+    <cellStyle name="Normal 6 3 3 3 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
+    <cellStyle name="Normal 6 3 3 3 2 2" xfId="653" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
+    <cellStyle name="Normal 6 3 3 3 2 3" xfId="654" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
+    <cellStyle name="Normal 6 3 3 3 3" xfId="115" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
+    <cellStyle name="Normal 6 3 3 3 4" xfId="112" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
+    <cellStyle name="Normal 6 3 3 4" xfId="647" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
+    <cellStyle name="Normal 6 3 3 4 2" xfId="317" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
+    <cellStyle name="Normal 6 3 3 4 3" xfId="316" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
+    <cellStyle name="Normal 6 3 3 5" xfId="646" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
+    <cellStyle name="Normal 6 3 3 6" xfId="648" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
+    <cellStyle name="Normal 6 3 4" xfId="550" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
+    <cellStyle name="Normal 6 3 4 2" xfId="160" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
+    <cellStyle name="Normal 6 3 4 2 2" xfId="470" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
+    <cellStyle name="Normal 6 3 4 2 3" xfId="471" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
+    <cellStyle name="Normal 6 3 4 3" xfId="164" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
+    <cellStyle name="Normal 6 3 4 4" xfId="155" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
+    <cellStyle name="Normal 6 3 5" xfId="551" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
+    <cellStyle name="Normal 6 3 5 2" xfId="493" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
+    <cellStyle name="Normal 6 3 5 2 2" xfId="53" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
+    <cellStyle name="Normal 6 3 5 2 3" xfId="52" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
+    <cellStyle name="Normal 6 3 5 3" xfId="492" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
+    <cellStyle name="Normal 6 3 5 4" xfId="491" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
+    <cellStyle name="Normal 6 3 6" xfId="552" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
+    <cellStyle name="Normal 6 3 6 2" xfId="323" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
+    <cellStyle name="Normal 6 3 6 2 2" xfId="153" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
+    <cellStyle name="Normal 6 3 6 2 3" xfId="154" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
+    <cellStyle name="Normal 6 3 6 3" xfId="324" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
+    <cellStyle name="Normal 6 3 6 4" xfId="322" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
+    <cellStyle name="Normal 6 3 7" xfId="553" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
+    <cellStyle name="Normal 6 3 7 2" xfId="111" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
+    <cellStyle name="Normal 6 3 7 2 2" xfId="347" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
+    <cellStyle name="Normal 6 3 7 2 3" xfId="346" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
+    <cellStyle name="Normal 6 3 7 3" xfId="110" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
+    <cellStyle name="Normal 6 3 7 4" xfId="109" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
+    <cellStyle name="Normal 6 3 8" xfId="501" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
+    <cellStyle name="Normal 6 3 8 2" xfId="305" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
+    <cellStyle name="Normal 6 3 8 3" xfId="306" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
+    <cellStyle name="Normal 6 3 9" xfId="502" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
+    <cellStyle name="Normal 6 4" xfId="311" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
+    <cellStyle name="Normal 6 4 10" xfId="100" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
+    <cellStyle name="Normal 6 4 2" xfId="92" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
+    <cellStyle name="Normal 6 4 2 2" xfId="140" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2" xfId="375" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 2" xfId="267" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="382" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 3" xfId="381" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 3" xfId="266" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 4" xfId="268" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3" xfId="395" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 2" xfId="480" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 2 2" xfId="187" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 2 3" xfId="188" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 3" xfId="481" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 4" xfId="484" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
+    <cellStyle name="Normal 6 4 2 2 4" xfId="402" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
+    <cellStyle name="Normal 6 4 2 2 4 2" xfId="429" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
+    <cellStyle name="Normal 6 4 2 2 4 3" xfId="428" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
+    <cellStyle name="Normal 6 4 2 2 5" xfId="401" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
+    <cellStyle name="Normal 6 4 2 2 6" xfId="379" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
+    <cellStyle name="Normal 6 4 2 3" xfId="139" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
+    <cellStyle name="Normal 6 4 2 3 2" xfId="587" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
+    <cellStyle name="Normal 6 4 2 3 2 2" xfId="655" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
+    <cellStyle name="Normal 6 4 2 3 2 3" xfId="656" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
+    <cellStyle name="Normal 6 4 2 3 3" xfId="588" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
+    <cellStyle name="Normal 6 4 2 3 4" xfId="591" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
+    <cellStyle name="Normal 6 4 2 4" xfId="138" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
+    <cellStyle name="Normal 6 4 2 4 2" xfId="623" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
+    <cellStyle name="Normal 6 4 2 4 2 2" xfId="605" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
+    <cellStyle name="Normal 6 4 2 4 2 3" xfId="604" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
+    <cellStyle name="Normal 6 4 2 4 3" xfId="622" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
+    <cellStyle name="Normal 6 4 2 4 4" xfId="621" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
+    <cellStyle name="Normal 6 4 2 5" xfId="137" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
+    <cellStyle name="Normal 6 4 2 5 2" xfId="184" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
+    <cellStyle name="Normal 6 4 2 5 3" xfId="185" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
+    <cellStyle name="Normal 6 4 2 6" xfId="136" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
+    <cellStyle name="Normal 6 4 2 7" xfId="135" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
+    <cellStyle name="Normal 6 4 3" xfId="91" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
+    <cellStyle name="Normal 6 4 3 2" xfId="342" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
+    <cellStyle name="Normal 6 4 3 2 2" xfId="200" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
+    <cellStyle name="Normal 6 4 3 2 2 2" xfId="127" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
+    <cellStyle name="Normal 6 4 3 2 2 3" xfId="128" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
+    <cellStyle name="Normal 6 4 3 2 3" xfId="201" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
+    <cellStyle name="Normal 6 4 3 2 4" xfId="204" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
+    <cellStyle name="Normal 6 4 3 3" xfId="343" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="Normal 6 4 3 3 2" xfId="643" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
+    <cellStyle name="Normal 6 4 3 3 2 2" xfId="298" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
+    <cellStyle name="Normal 6 4 3 3 2 3" xfId="297" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
+    <cellStyle name="Normal 6 4 3 3 3" xfId="642" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
+    <cellStyle name="Normal 6 4 3 3 4" xfId="583" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
+    <cellStyle name="Normal 6 4 3 4" xfId="340" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
+    <cellStyle name="Normal 6 4 3 4 2" xfId="444" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
+    <cellStyle name="Normal 6 4 3 4 3" xfId="445" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
+    <cellStyle name="Normal 6 4 3 5" xfId="341" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
+    <cellStyle name="Normal 6 4 3 6" xfId="339" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
+    <cellStyle name="Normal 6 4 4" xfId="441" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
+    <cellStyle name="Normal 6 4 4 2" xfId="292" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
+    <cellStyle name="Normal 6 4 4 2 2" xfId="247" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
+    <cellStyle name="Normal 6 4 4 2 3" xfId="246" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
+    <cellStyle name="Normal 6 4 4 3" xfId="412" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
+    <cellStyle name="Normal 6 4 4 4" xfId="293" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
+    <cellStyle name="Normal 6 4 5" xfId="440" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
+    <cellStyle name="Normal 6 4 5 2" xfId="460" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
+    <cellStyle name="Normal 6 4 5 2 2" xfId="517" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
+    <cellStyle name="Normal 6 4 5 2 3" xfId="520" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
+    <cellStyle name="Normal 6 4 5 3" xfId="461" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
+    <cellStyle name="Normal 6 4 5 4" xfId="462" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
+    <cellStyle name="Normal 6 4 6" xfId="88" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
+    <cellStyle name="Normal 6 4 6 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
+    <cellStyle name="Normal 6 4 6 2 2" xfId="595" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
+    <cellStyle name="Normal 6 4 6 2 3" xfId="594" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
+    <cellStyle name="Normal 6 4 6 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
+    <cellStyle name="Normal 6 4 6 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
+    <cellStyle name="Normal 6 4 7" xfId="87" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
+    <cellStyle name="Normal 6 4 7 2" xfId="221" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
+    <cellStyle name="Normal 6 4 7 2 2" xfId="403" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
+    <cellStyle name="Normal 6 4 7 2 3" xfId="404" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
+    <cellStyle name="Normal 6 4 7 3" xfId="222" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
+    <cellStyle name="Normal 6 4 7 4" xfId="224" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
+    <cellStyle name="Normal 6 4 8" xfId="97" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
+    <cellStyle name="Normal 6 4 8 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
+    <cellStyle name="Normal 6 4 8 3" xfId="380" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
+    <cellStyle name="Normal 6 4 9" xfId="96" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
+    <cellStyle name="Normal 6 5" xfId="310" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
+    <cellStyle name="Normal 6 5 2" xfId="285" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
+    <cellStyle name="Normal 6 5 2 2" xfId="534" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2" xfId="182" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 2" xfId="258" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 2 2" xfId="546" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 2 3" xfId="547" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 3" xfId="259" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 4" xfId="261" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3" xfId="417" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 2" xfId="302" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 2 2" xfId="107" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 2 3" xfId="106" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 3" xfId="301" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 4" xfId="79" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
+    <cellStyle name="Normal 6 5 2 2 4" xfId="253" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
+    <cellStyle name="Normal 6 5 2 2 4 2" xfId="419" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
+    <cellStyle name="Normal 6 5 2 2 4 3" xfId="420" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
+    <cellStyle name="Normal 6 5 2 2 5" xfId="254" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
+    <cellStyle name="Normal 6 5 2 2 6" xfId="192" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
+    <cellStyle name="Normal 6 5 2 3" xfId="535" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
+    <cellStyle name="Normal 6 5 2 3 2" xfId="649" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
+    <cellStyle name="Normal 6 5 2 3 2 2" xfId="370" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
+    <cellStyle name="Normal 6 5 2 3 2 3" xfId="369" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
+    <cellStyle name="Normal 6 5 2 3 3" xfId="70" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
+    <cellStyle name="Normal 6 5 2 3 4" xfId="276" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
+    <cellStyle name="Normal 6 5 2 4" xfId="532" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
+    <cellStyle name="Normal 6 5 2 4 2" xfId="518" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
+    <cellStyle name="Normal 6 5 2 4 2 2" xfId="633" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
+    <cellStyle name="Normal 6 5 2 4 2 3" xfId="634" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
+    <cellStyle name="Normal 6 5 2 4 3" xfId="519" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
+    <cellStyle name="Normal 6 5 2 4 4" xfId="514" xr:uid="{00000000-0005-0000-0000-0000A1010000}"/>
+    <cellStyle name="Normal 6 5 2 5" xfId="447" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
+    <cellStyle name="Normal 6 5 2 5 2" xfId="304" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
+    <cellStyle name="Normal 6 5 2 5 3" xfId="303" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
+    <cellStyle name="Normal 6 5 2 6" xfId="530" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
+    <cellStyle name="Normal 6 5 2 7" xfId="531" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
+    <cellStyle name="Normal 6 5 3" xfId="286" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
+    <cellStyle name="Normal 6 5 3 2" xfId="321" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
+    <cellStyle name="Normal 6 5 3 2 2" xfId="134" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
+    <cellStyle name="Normal 6 5 3 2 2 2" xfId="600" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
+    <cellStyle name="Normal 6 5 3 2 2 3" xfId="599" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
+    <cellStyle name="Normal 6 5 3 2 3" xfId="229" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
+    <cellStyle name="Normal 6 5 3 2 4" xfId="472" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
+    <cellStyle name="Normal 6 5 3 3" xfId="320" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
+    <cellStyle name="Normal 6 5 3 3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
+    <cellStyle name="Normal 6 5 3 3 2 2" xfId="423" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
+    <cellStyle name="Normal 6 5 3 3 2 3" xfId="424" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
+    <cellStyle name="Normal 6 5 3 3 3" xfId="34" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
+    <cellStyle name="Normal 6 5 3 3 4" xfId="9" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
+    <cellStyle name="Normal 6 5 3 4" xfId="319" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
+    <cellStyle name="Normal 6 5 3 4 2" xfId="94" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
+    <cellStyle name="Normal 6 5 3 4 3" xfId="93" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
+    <cellStyle name="Normal 6 5 3 5" xfId="318" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
+    <cellStyle name="Normal 6 5 3 6" xfId="525" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
+    <cellStyle name="Normal 6 5 4" xfId="283" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
+    <cellStyle name="Normal 6 5 4 2" xfId="582" xr:uid="{00000000-0005-0000-0000-0000BA010000}"/>
+    <cellStyle name="Normal 6 5 4 2 2" xfId="478" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
+    <cellStyle name="Normal 6 5 4 2 3" xfId="639" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
+    <cellStyle name="Normal 6 5 4 3" xfId="197" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
+    <cellStyle name="Normal 6 5 4 4" xfId="584" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
+    <cellStyle name="Normal 6 5 5" xfId="284" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
+    <cellStyle name="Normal 6 5 5 2" xfId="387" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
+    <cellStyle name="Normal 6 5 5 2 2" xfId="119" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
+    <cellStyle name="Normal 6 5 5 2 3" xfId="33" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
+    <cellStyle name="Normal 6 5 5 3" xfId="386" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
+    <cellStyle name="Normal 6 5 5 4" xfId="388" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
+    <cellStyle name="Normal 6 5 6" xfId="281" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
+    <cellStyle name="Normal 6 5 6 2" xfId="74" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
+    <cellStyle name="Normal 6 5 6 3" xfId="356" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
+    <cellStyle name="Normal 6 5 7" xfId="282" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
+    <cellStyle name="Normal 6 5 8" xfId="280" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
+    <cellStyle name="Normal 6 6" xfId="313" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
+    <cellStyle name="Normal 6 6 2" xfId="326" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
+    <cellStyle name="Normal 6 6 2 2" xfId="245" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2" xfId="64" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 2" xfId="618" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 2 2" xfId="39" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 2 3" xfId="515" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 3" xfId="617" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 4" xfId="619" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3" xfId="113" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 2" xfId="116" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 2 2" xfId="456" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 2 3" xfId="457" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 3" xfId="296" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 4" xfId="176" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
+    <cellStyle name="Normal 6 6 2 2 4" xfId="80" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
+    <cellStyle name="Normal 6 6 2 2 4 2" xfId="199" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
+    <cellStyle name="Normal 6 6 2 2 4 3" xfId="198" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
+    <cellStyle name="Normal 6 6 2 2 5" xfId="77" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
+    <cellStyle name="Normal 6 6 2 2 6" xfId="129" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
+    <cellStyle name="Normal 6 6 2 3" xfId="163" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
+    <cellStyle name="Normal 6 6 2 3 2" xfId="662" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
+    <cellStyle name="Normal 6 6 2 3 2 2" xfId="278" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
+    <cellStyle name="Normal 6 6 2 3 2 3" xfId="279" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
+    <cellStyle name="Normal 6 6 2 3 3" xfId="1" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
+    <cellStyle name="Normal 6 6 2 3 4" xfId="2" xr:uid="{00000000-0005-0000-0000-0000E3010000}"/>
+    <cellStyle name="Normal 6 6 2 4" xfId="586" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
+    <cellStyle name="Normal 6 6 2 4 2" xfId="581" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
+    <cellStyle name="Normal 6 6 2 4 2 2" xfId="383" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
+    <cellStyle name="Normal 6 6 2 4 2 3" xfId="516" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
+    <cellStyle name="Normal 6 6 2 4 3" xfId="580" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
+    <cellStyle name="Normal 6 6 2 4 4" xfId="579" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
+    <cellStyle name="Normal 6 6 2 5" xfId="159" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
+    <cellStyle name="Normal 6 6 2 5 2" xfId="141" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
+    <cellStyle name="Normal 6 6 2 5 3" xfId="142" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
+    <cellStyle name="Normal 6 6 2 6" xfId="162" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
+    <cellStyle name="Normal 6 6 2 7" xfId="161" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
+    <cellStyle name="Normal 6 6 3" xfId="325" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
+    <cellStyle name="Normal 6 6 3 2" xfId="374" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
+    <cellStyle name="Normal 6 6 3 2 2" xfId="275" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
+    <cellStyle name="Normal 6 6 3 2 2 2" xfId="410" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
+    <cellStyle name="Normal 6 6 3 2 2 3" xfId="411" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
+    <cellStyle name="Normal 6 6 3 2 3" xfId="362" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
+    <cellStyle name="Normal 6 6 3 2 4" xfId="277" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
+    <cellStyle name="Normal 6 6 3 3" xfId="186" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
+    <cellStyle name="Normal 6 6 3 3 2" xfId="105" xr:uid="{00000000-0005-0000-0000-0000F7010000}"/>
+    <cellStyle name="Normal 6 6 3 3 2 2" xfId="300" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
+    <cellStyle name="Normal 6 6 3 3 2 3" xfId="299" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
+    <cellStyle name="Normal 6 6 3 3 3" xfId="104" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
+    <cellStyle name="Normal 6 6 3 3 4" xfId="574" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
+    <cellStyle name="Normal 6 6 3 4" xfId="371" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
+    <cellStyle name="Normal 6 6 3 4 2" xfId="391" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
+    <cellStyle name="Normal 6 6 3 4 3" xfId="392" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
+    <cellStyle name="Normal 6 6 3 5" xfId="372" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
+    <cellStyle name="Normal 6 6 3 6" xfId="373" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
+    <cellStyle name="Normal 6 6 4" xfId="108" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
+    <cellStyle name="Normal 6 6 4 2" xfId="435" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
+    <cellStyle name="Normal 6 6 4 2 2" xfId="433" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
+    <cellStyle name="Normal 6 6 4 2 3" xfId="432" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
+    <cellStyle name="Normal 6 6 4 3" xfId="434" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
+    <cellStyle name="Normal 6 6 4 4" xfId="438" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
+    <cellStyle name="Normal 6 6 5" xfId="585" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
+    <cellStyle name="Normal 6 6 5 2" xfId="596" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
+    <cellStyle name="Normal 6 6 5 2 2" xfId="554" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
+    <cellStyle name="Normal 6 6 5 2 3" xfId="555" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
+    <cellStyle name="Normal 6 6 5 3" xfId="597" xr:uid="{00000000-0005-0000-0000-00000B020000}"/>
+    <cellStyle name="Normal 6 6 5 4" xfId="598" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
+    <cellStyle name="Normal 6 6 6" xfId="616" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
+    <cellStyle name="Normal 6 6 6 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
+    <cellStyle name="Normal 6 6 6 3" xfId="28" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
+    <cellStyle name="Normal 6 6 7" xfId="507" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
+    <cellStyle name="Normal 6 6 8" xfId="513" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
+    <cellStyle name="Normal 6 7" xfId="312" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
+    <cellStyle name="Normal 6 7 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
+    <cellStyle name="Normal 6 7 2 2" xfId="610" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 2" xfId="615" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 2 2" xfId="243" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 2 3" xfId="244" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 3" xfId="120" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 4" xfId="562" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 2" xfId="358" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 2 2" xfId="390" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 2 3" xfId="144" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 3" xfId="357" xr:uid="{00000000-0005-0000-0000-00001F020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 4" xfId="359" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
+    <cellStyle name="Normal 6 7 2 2 4" xfId="124" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
+    <cellStyle name="Normal 6 7 2 2 4 2" xfId="170" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
+    <cellStyle name="Normal 6 7 2 2 4 3" xfId="171" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
+    <cellStyle name="Normal 6 7 2 2 5" xfId="125" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
+    <cellStyle name="Normal 6 7 2 2 6" xfId="126" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
+    <cellStyle name="Normal 6 7 2 3" xfId="611" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
+    <cellStyle name="Normal 6 7 2 3 2" xfId="572" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
+    <cellStyle name="Normal 6 7 2 3 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
+    <cellStyle name="Normal 6 7 2 3 2 3" xfId="327" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
+    <cellStyle name="Normal 6 7 2 3 3" xfId="571" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
+    <cellStyle name="Normal 6 7 2 3 4" xfId="573" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
+    <cellStyle name="Normal 6 7 2 4" xfId="606" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
+    <cellStyle name="Normal 6 7 2 4 2" xfId="272" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
+    <cellStyle name="Normal 6 7 2 4 2 2" xfId="179" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
+    <cellStyle name="Normal 6 7 2 4 2 3" xfId="536" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
+    <cellStyle name="Normal 6 7 2 4 3" xfId="273" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
+    <cellStyle name="Normal 6 7 2 4 4" xfId="271" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
+    <cellStyle name="Normal 6 7 2 5" xfId="607" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
+    <cellStyle name="Normal 6 7 2 5 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000033020000}"/>
+    <cellStyle name="Normal 6 7 2 5 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
+    <cellStyle name="Normal 6 7 2 6" xfId="608" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
+    <cellStyle name="Normal 6 7 2 7" xfId="609" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
+    <cellStyle name="Normal 6 7 3" xfId="66" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
+    <cellStyle name="Normal 6 7 3 2" xfId="409" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
+    <cellStyle name="Normal 6 7 3 2 2" xfId="476" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
+    <cellStyle name="Normal 6 7 3 2 2 2" xfId="353" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
+    <cellStyle name="Normal 6 7 3 2 2 3" xfId="352" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
+    <cellStyle name="Normal 6 7 3 2 3" xfId="475" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
+    <cellStyle name="Normal 6 7 3 2 4" xfId="477" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
+    <cellStyle name="Normal 6 7 3 3" xfId="418" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
+    <cellStyle name="Normal 6 7 3 3 2" xfId="650" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
+    <cellStyle name="Normal 6 7 3 3 2 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
+    <cellStyle name="Normal 6 7 3 3 2 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
+    <cellStyle name="Normal 6 7 3 3 3" xfId="651" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
+    <cellStyle name="Normal 6 7 3 3 4" xfId="652" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
+    <cellStyle name="Normal 6 7 3 4" xfId="414" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
+    <cellStyle name="Normal 6 7 3 4 2" xfId="563" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
+    <cellStyle name="Normal 6 7 3 4 3" xfId="620" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
+    <cellStyle name="Normal 6 7 3 5" xfId="413" xr:uid="{00000000-0005-0000-0000-000047020000}"/>
+    <cellStyle name="Normal 6 7 3 6" xfId="407" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
+    <cellStyle name="Normal 6 7 4" xfId="60" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
+    <cellStyle name="Normal 6 7 4 2" xfId="166" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
+    <cellStyle name="Normal 6 7 4 2 2" xfId="509" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
+    <cellStyle name="Normal 6 7 4 2 3" xfId="510" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
+    <cellStyle name="Normal 6 7 4 3" xfId="490" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
+    <cellStyle name="Normal 6 7 4 4" xfId="494" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
+    <cellStyle name="Normal 6 7 5" xfId="61" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
+    <cellStyle name="Normal 6 7 5 2" xfId="638" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
+    <cellStyle name="Normal 6 7 5 2 2" xfId="152" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
+    <cellStyle name="Normal 6 7 5 2 3" xfId="38" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
+    <cellStyle name="Normal 6 7 5 3" xfId="637" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
+    <cellStyle name="Normal 6 7 5 4" xfId="641" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
+    <cellStyle name="Normal 6 7 6" xfId="62" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
+    <cellStyle name="Normal 6 7 6 2" xfId="415" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
+    <cellStyle name="Normal 6 7 6 3" xfId="416" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
+    <cellStyle name="Normal 6 7 7" xfId="63" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
+    <cellStyle name="Normal 6 7 8" xfId="59" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
+    <cellStyle name="Normal 6 8" xfId="308" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
+    <cellStyle name="Normal 6 8 2" xfId="364" xr:uid="{00000000-0005-0000-0000-00005B020000}"/>
+    <cellStyle name="Normal 6 8 2 2" xfId="146" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
+    <cellStyle name="Normal 6 8 2 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
+    <cellStyle name="Normal 6 8 2 2 2 2" xfId="345" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
+    <cellStyle name="Normal 6 8 2 2 2 3" xfId="344" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
+    <cellStyle name="Normal 6 8 2 2 3" xfId="18" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
+    <cellStyle name="Normal 6 8 2 2 4" xfId="575" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
+    <cellStyle name="Normal 6 8 2 3" xfId="145" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
+    <cellStyle name="Normal 6 8 2 3 2" xfId="240" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
+    <cellStyle name="Normal 6 8 2 3 2 2" xfId="202" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
+    <cellStyle name="Normal 6 8 2 3 2 3" xfId="203" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
+    <cellStyle name="Normal 6 8 2 3 3" xfId="241" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
+    <cellStyle name="Normal 6 8 2 3 4" xfId="239" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
+    <cellStyle name="Normal 6 8 2 4" xfId="149" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
+    <cellStyle name="Normal 6 8 2 4 2" xfId="625" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
+    <cellStyle name="Normal 6 8 2 4 3" xfId="624" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
+    <cellStyle name="Normal 6 8 2 5" xfId="148" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
+    <cellStyle name="Normal 6 8 2 6" xfId="147" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
+    <cellStyle name="Normal 6 8 3" xfId="363" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
+    <cellStyle name="Normal 6 8 3 2" xfId="350" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
+    <cellStyle name="Normal 6 8 3 2 2" xfId="488" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
+    <cellStyle name="Normal 6 8 3 2 3" xfId="489" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
+    <cellStyle name="Normal 6 8 3 3" xfId="351" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
+    <cellStyle name="Normal 6 8 3 4" xfId="354" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
+    <cellStyle name="Normal 6 8 4" xfId="368" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
+    <cellStyle name="Normal 6 8 4 2" xfId="565" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
+    <cellStyle name="Normal 6 8 4 2 2" xfId="165" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
+    <cellStyle name="Normal 6 8 4 2 3" xfId="446" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
+    <cellStyle name="Normal 6 8 4 3" xfId="564" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
+    <cellStyle name="Normal 6 8 4 4" xfId="559" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
+    <cellStyle name="Normal 6 8 5" xfId="367" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
+    <cellStyle name="Normal 6 8 5 2" xfId="102" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
+    <cellStyle name="Normal 6 8 5 3" xfId="103" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
+    <cellStyle name="Normal 6 8 6" xfId="366" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
+    <cellStyle name="Normal 6 8 7" xfId="365" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
+    <cellStyle name="Normal 6 9" xfId="307" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
+    <cellStyle name="Normal 6 9 2" xfId="537" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
+    <cellStyle name="Normal 6 9 2 2" xfId="215" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
+    <cellStyle name="Normal 6 9 2 2 2" xfId="264" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
+    <cellStyle name="Normal 6 9 2 2 3" xfId="265" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
+    <cellStyle name="Normal 6 9 2 3" xfId="566" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
+    <cellStyle name="Normal 6 9 2 4" xfId="217" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
+    <cellStyle name="Normal 6 9 3" xfId="538" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
+    <cellStyle name="Normal 6 9 3 2" xfId="658" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
+    <cellStyle name="Normal 6 9 3 2 2" xfId="426" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
+    <cellStyle name="Normal 6 9 3 2 3" xfId="425" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
+    <cellStyle name="Normal 6 9 3 3" xfId="657" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
+    <cellStyle name="Normal 6 9 3 4" xfId="659" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
+    <cellStyle name="Normal 6 9 4" xfId="540" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
+    <cellStyle name="Normal 6 9 4 2" xfId="640" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
+    <cellStyle name="Normal 6 9 4 3" xfId="567" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
+    <cellStyle name="Normal 6 9 5" xfId="541" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
+    <cellStyle name="Normal 6 9 6" xfId="539" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
+    <cellStyle name="Normal 7" xfId="452" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
+    <cellStyle name="Normal 7 2" xfId="529" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
+    <cellStyle name="Normal 8" xfId="455" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
+    <cellStyle name="Normal 8 2" xfId="576" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
+    <cellStyle name="Normal 9" xfId="454" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
+    <cellStyle name="Normal 9 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
+    <cellStyle name="Percent 2" xfId="269" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
+    <cellStyle name="Percent 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-000097020000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2169,7 +2182,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -2367,19 +2380,19 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B5:B6">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B5:B6" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -2390,17 +2403,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AC15"/>
+  <dimension ref="A1:AC19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2897,18 +2910,102 @@
         <v>95</v>
       </c>
     </row>
+    <row r="16" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="O16" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="Q16" s="41"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="41"/>
+      <c r="T16" s="41"/>
+      <c r="U16" s="41"/>
+      <c r="V16" s="41"/>
+    </row>
+    <row r="17" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="O17" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="41"/>
+      <c r="V17" s="41"/>
+    </row>
+    <row r="18" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="O18" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="41"/>
+      <c r="U18" s="41"/>
+      <c r="V18" s="41"/>
+    </row>
+    <row r="19" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="O19" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="41"/>
+      <c r="T19" s="41"/>
+      <c r="U19" s="41"/>
+      <c r="V19" s="41"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E3:O4 Q3:Q8">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E3:O4 Q3:Q8" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1:C2"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E5:P8 Q5:Q7">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1:C2" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="E5:P8 Q5:Q7" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C3:C1048576">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C3:C1048576" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2919,7 +3016,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>

</xml_diff>

<commit_message>
Implement IPT for all age groups
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C3F294-080F-4C9B-85E7-00F9616C1AA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A563A9B6-8851-40B9-AFA8-0A6338E9088B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15340" windowHeight="5480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
   <si>
     <t>parameter</t>
   </si>
@@ -235,6 +235,66 @@
   </si>
   <si>
     <t>econ_startupcost_treatment_support_relative</t>
+  </si>
+  <si>
+    <t>scenario_8</t>
+  </si>
+  <si>
+    <t>int_perc_ipt_age15to25</t>
+  </si>
+  <si>
+    <t>scenario_9</t>
+  </si>
+  <si>
+    <t>int_perc_ipt_age25up</t>
+  </si>
+  <si>
+    <t>scenario_10</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>econ_startupduration_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>econ_saturation_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ipt_age15to25</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_ipt_age15to25</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ipt_age15to25</t>
+  </si>
+  <si>
+    <t>econ_startupduration_ipt_age15to25</t>
+  </si>
+  <si>
+    <t>econ_saturation_ipt_age15to25</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ipt_age25up</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_ipt_age25up</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ipt_age25up</t>
+  </si>
+  <si>
+    <t>econ_startupduration_ipt_age25up</t>
+  </si>
+  <si>
+    <t>econ_saturation_ipt_age25up</t>
   </si>
 </sst>
 </file>
@@ -2256,21 +2316,21 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.54296875" style="56" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" style="57" customWidth="1"/>
-    <col min="3" max="8" width="9.08984375" style="49" customWidth="1"/>
-    <col min="9" max="16384" width="9.08984375" style="49"/>
+    <col min="1" max="1" width="51.5703125" style="56" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="57" customWidth="1"/>
+    <col min="3" max="8" width="9.140625" style="49" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -2278,7 +2338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>2</v>
       </c>
@@ -2286,7 +2346,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
         <v>3</v>
       </c>
@@ -2294,7 +2354,7 @@
         <v>9.9999999999999978E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>4</v>
       </c>
@@ -2302,7 +2362,7 @@
         <v>1845.0101752600381</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>5</v>
       </c>
@@ -2310,7 +2370,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
         <v>6</v>
       </c>
@@ -2318,7 +2378,7 @@
         <v>892000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
         <v>7</v>
       </c>
@@ -2332,7 +2392,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2340,7 +2400,7 @@
         <v>0.62465901134638702</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2348,7 +2408,7 @@
         <v>0.72626503054609337</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2356,7 +2416,7 @@
         <v>2.816856563164909</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2364,7 +2424,7 @@
         <v>0.29026946983549362</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="61" t="s">
         <v>12</v>
       </c>
@@ -2372,7 +2432,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="13" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>47</v>
       </c>
@@ -2384,7 +2444,7 @@
       <c r="D13" s="64"/>
       <c r="E13" s="65"/>
     </row>
-    <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="63" t="s">
         <v>48</v>
       </c>
@@ -2396,7 +2456,7 @@
       <c r="D14" s="64"/>
       <c r="E14" s="65"/>
     </row>
-    <row r="15" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
         <v>49</v>
       </c>
@@ -2408,7 +2468,7 @@
       <c r="D15" s="64"/>
       <c r="E15" s="65"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="66" t="s">
         <v>45</v>
       </c>
@@ -2416,7 +2476,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="66" t="s">
         <v>50</v>
       </c>
@@ -2424,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="56" t="s">
         <v>44</v>
       </c>
@@ -2432,7 +2492,7 @@
         <v>540.1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
         <v>51</v>
       </c>
@@ -2440,7 +2500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
         <v>69</v>
       </c>
@@ -2448,7 +2508,7 @@
         <v>540.1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
         <v>70</v>
       </c>
@@ -2456,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="66" t="s">
         <v>52</v>
       </c>
@@ -2464,7 +2524,7 @@
         <v>1153.5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="66" t="s">
         <v>53</v>
       </c>
@@ -2472,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
         <v>54</v>
       </c>
@@ -2480,7 +2540,7 @@
         <v>127.11499999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
         <v>55</v>
       </c>
@@ -2488,7 +2548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="66" t="s">
         <v>56</v>
       </c>
@@ -2496,7 +2556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="66" t="s">
         <v>57</v>
       </c>
@@ -2504,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="68" t="s">
         <v>59</v>
       </c>
@@ -2512,7 +2572,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="68" t="s">
         <v>60</v>
       </c>
@@ -2520,7 +2580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="68" t="s">
         <v>61</v>
       </c>
@@ -2528,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="68" t="s">
         <v>62</v>
       </c>
@@ -2536,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="68" t="s">
         <v>63</v>
       </c>
@@ -2544,7 +2604,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="68" t="s">
         <v>64</v>
       </c>
@@ -2552,7 +2612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="68" t="s">
         <v>65</v>
       </c>
@@ -2560,7 +2620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="68" t="s">
         <v>66</v>
       </c>
@@ -2568,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="68" t="s">
         <v>67</v>
       </c>
@@ -2576,12 +2636,132 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="68" t="s">
         <v>68</v>
       </c>
       <c r="B37" s="68">
         <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="68">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="68" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="68">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="68">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="68">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="68">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" s="68">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -2613,36 +2793,38 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AC16"/>
+  <dimension ref="A1:AC18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U16" sqref="U16"/>
+      <selection pane="bottomRight" activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="2" customWidth="1"/>
     <col min="4" max="4" width="11" style="54" customWidth="1"/>
-    <col min="5" max="5" width="7.36328125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="7.453125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="7.42578125" style="1" customWidth="1"/>
     <col min="8" max="11" width="7" style="1" customWidth="1"/>
-    <col min="12" max="13" width="7.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="7.90625" style="1" customWidth="1"/>
+    <col min="12" max="13" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="7.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" style="1" customWidth="1"/>
-    <col min="18" max="20" width="14.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.453125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="28" width="9.08984375" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.08984375" style="1"/>
+    <col min="18" max="20" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.85546875" style="1" customWidth="1"/>
+    <col min="26" max="28" width="9.140625" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -2712,8 +2894,17 @@
       <c r="W1" s="45" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" s="60" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="X1" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y1" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" s="45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>24</v>
       </c>
@@ -2724,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>26</v>
       </c>
@@ -2753,8 +2944,11 @@
       <c r="V3" s="37">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Z3" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>27</v>
       </c>
@@ -2773,8 +2967,14 @@
       <c r="T4" s="37"/>
       <c r="U4" s="37"/>
       <c r="V4" s="37"/>
-    </row>
-    <row r="5" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Y4" s="6">
+        <v>100</v>
+      </c>
+      <c r="Z4" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>28</v>
       </c>
@@ -2795,7 +2995,7 @@
       <c r="U5" s="39"/>
       <c r="V5" s="39"/>
     </row>
-    <row r="6" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>30</v>
       </c>
@@ -2819,7 +3019,7 @@
       <c r="U6" s="40"/>
       <c r="V6" s="40"/>
     </row>
-    <row r="7" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>31</v>
       </c>
@@ -2846,7 +3046,7 @@
       <c r="U7" s="40"/>
       <c r="V7" s="40"/>
     </row>
-    <row r="8" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>32</v>
       </c>
@@ -2865,9 +3065,7 @@
         <v>0.01</v>
       </c>
       <c r="Q8" s="42"/>
-      <c r="R8" s="42">
-        <v>96</v>
-      </c>
+      <c r="R8" s="42"/>
       <c r="S8" s="42"/>
       <c r="T8" s="42"/>
       <c r="U8" s="42"/>
@@ -2875,7 +3073,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>33</v>
       </c>
@@ -2916,7 +3114,7 @@
       <c r="AB9" s="23"/>
       <c r="AC9" s="23"/>
     </row>
-    <row r="10" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>34</v>
       </c>
@@ -2959,7 +3157,7 @@
       <c r="AB10" s="23"/>
       <c r="AC10" s="23"/>
     </row>
-    <row r="11" spans="1:29" s="32" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>35</v>
       </c>
@@ -2982,7 +3180,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:29" s="32" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>36</v>
       </c>
@@ -3003,7 +3201,7 @@
       </c>
       <c r="V12" s="38"/>
     </row>
-    <row r="13" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>37</v>
       </c>
@@ -3051,7 +3249,7 @@
       <c r="U13" s="44"/>
       <c r="V13" s="44"/>
     </row>
-    <row r="14" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>38</v>
       </c>
@@ -3093,7 +3291,7 @@
       <c r="U14" s="41"/>
       <c r="V14" s="41"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="62" t="s">
         <v>46</v>
       </c>
@@ -3110,15 +3308,37 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>58</v>
       </c>
       <c r="N16" s="1">
         <v>0.01</v>
       </c>
+      <c r="R16" s="1">
+        <v>100</v>
+      </c>
       <c r="V16" s="1">
         <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="X17" s="1">
+        <v>100</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3153,9 +3373,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -3169,7 +3389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -3180,7 +3400,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>

</xml_diff>